<commit_message>
- 2020 results final
</commit_message>
<xml_diff>
--- a/processor/config2020.xlsx
+++ b/processor/config2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Data\Problems\vkct\processor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F549D7-3E89-4E93-A247-1222E87DED77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC56BFD0-91AC-4CFF-AE8E-89A2A9CB0660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="-60" windowWidth="28920" windowHeight="18120" tabRatio="937" firstSheet="4" activeTab="14" xr2:uid="{15338A40-4FCA-4B48-85DC-9A39AA2E7524}"/>
+    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="16890" tabRatio="937" xr2:uid="{15338A40-4FCA-4B48-85DC-9A39AA2E7524}"/>
   </bookViews>
   <sheets>
     <sheet name="Kategorie" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="65">
   <si>
     <t>Rok:</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Z2</t>
+  </si>
+  <si>
+    <t>..\2020\05-plostina\plostina2020.xlsx</t>
   </si>
 </sst>
 </file>
@@ -636,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F60167-74EE-4847-B777-F54D2D3F9AAF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1090,1189 +1093,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66DD3EB-1418-4AD7-AF94-FBBA9B37CCA7}">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536DB9BF-9270-4AA0-8EA3-C2E9A08212FE}">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946E38EF-5743-4933-9DDC-13FFB0014327}">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36456C0-7065-486E-8B2F-B411D84D34E2}">
-  <dimension ref="A1:N5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC10038-95CC-4975-AE20-40C87AC8AF81}">
-  <dimension ref="A1:N6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC34F1C-98BB-4F0C-8303-1E228B91F05E}">
-  <dimension ref="A1:N6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD4F9F6-A3DB-4EB0-B5CD-B5C06460778A}">
-  <dimension ref="A1:N6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D04EC5F-3248-47A8-8EC7-2E949A0B770F}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2327,10 +1147,10 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -2353,10 +1173,10 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -2379,7 +1199,7 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2399,36 +1219,36 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>7</v>
@@ -2454,8 +1274,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DBF4A4-BFA5-47D1-88BF-341A86C1E640}">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{536DB9BF-9270-4AA0-8EA3-C2E9A08212FE}">
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2510,10 +1330,10 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -2536,10 +1356,10 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -2562,7 +1382,562 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>27</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946E38EF-5743-4933-9DDC-13FFB0014327}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36456C0-7065-486E-8B2F-B411D84D34E2}">
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC10038-95CC-4975-AE20-40C87AC8AF81}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2585,7 +1960,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2611,8 +1986,844 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC34F1C-98BB-4F0C-8303-1E228B91F05E}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDD4F9F6-A3DB-4EB0-B5CD-B5C06460778A}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D04EC5F-3248-47A8-8EC7-2E949A0B770F}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DBF4A4-BFA5-47D1-88BF-341A86C1E640}">
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
         <v>33</v>
       </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
       <c r="C6">
         <v>7</v>
       </c>
@@ -2629,6 +2840,32 @@
         <v>14</v>
       </c>
       <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2639,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBE0CB4-6079-4D52-8B87-706BE18C11DA}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2790,6 +3027,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2798,7 +3061,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032E0053-8426-48C9-B2BD-0093B4F61388}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -2948,6 +3211,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2955,10 +3244,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133430E9-4ED1-4C6D-8E2B-9EA6F1CD5FA9}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,6 +3394,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3112,10 +3427,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F88C79-E3DD-4029-A83E-4EDCB62AFB21}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3262,6 +3577,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3269,10 +3610,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8F5731-8725-4499-A7BF-4B334BF8702B}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3419,6 +3760,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3426,10 +3793,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BB204B-3660-4703-9383-5A8A01119918}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3576,6 +3943,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3583,10 +3976,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DAA0746-7BD2-400D-8377-89715DC1C86E}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3733,6 +4126,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3740,10 +4159,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B030A4-A1C4-4E81-B505-FEA2C1F1BD9C}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3890,6 +4309,32 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>